<commit_message>
Modified inventory file to better organize data for search improvement
</commit_message>
<xml_diff>
--- a/Equipment_Registration_App/Equipment_Registration_App/alm_hardware.xlsx
+++ b/Equipment_Registration_App/Equipment_Registration_App/alm_hardware.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andresfelipe.perez\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andresfelipe.perez\PycharmProjects\Equipment_Registration_App\Equipment_Registration_App\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFBF8A1C-8AE3-4C6D-AA83-AC83587D2437}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64D72F21-3B65-4FB1-88DD-99178747C95E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14460" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Page 1" sheetId="1" r:id="rId1"/>
@@ -12638,8 +12638,8 @@
   <dimension ref="A1:E2300"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G20" sqref="G20"/>
+      <pane ySplit="1" topLeftCell="A164" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="29.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -51752,7 +51752,11 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E2300" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:E2300" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E2300">
+      <sortCondition descending="1" ref="C1:C2300"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
     <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;8&amp;K737373 Asurion_Internal_Use_Only</oddFooter>

</xml_diff>